<commit_message>
Day - 7 All Passed
</commit_message>
<xml_diff>
--- a/IxigoTrains/src/test/resources/ExcelData/Book4.xlsx
+++ b/IxigoTrains/src/test/resources/ExcelData/Book4.xlsx
@@ -3,75 +3,29 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://capgemini-my.sharepoint.com/personal/vanga-srinivasa-rao_vanga-srinivasa-rao_capgemini_com/Documents/Desktop/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="14_{A0571C43-3268-4D4D-B0B8-7611AE3A15F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6073E10-72EB-4486-B357-DAC3029E93A8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{175708F4-A20D-44A6-83FF-97B63BDA1B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{0270D0DF-FD8A-46BE-9582-0B80E53E6909}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{0270D0DF-FD8A-46BE-9582-0B80E53E6909}"/>
   </bookViews>
   <sheets>
-    <sheet name="TrainChart" sheetId="1" r:id="rId1"/>
-    <sheet name="PNR" sheetId="2" r:id="rId2"/>
+    <sheet name="PNR" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:L11"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>New Delhi (NDLS)</t>
-  </si>
-  <si>
-    <t>Lokmanyatilak T (LTT)</t>
-  </si>
-  <si>
-    <t>From</t>
-  </si>
-  <si>
-    <t>To</t>
-  </si>
-  <si>
-    <t>Howrah Jn (HWH)</t>
-  </si>
-  <si>
-    <t>Ahmedabad Jn (ADI)</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF17181C"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -97,12 +51,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -121,10 +71,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -443,52 +389,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0A9DEE7-CED7-465F-AB64-8C121C10FBCA}">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="22.453125" customWidth="1"/>
-    <col min="2" max="2" width="22.7265625" customWidth="1"/>
-    <col min="3" max="3" width="19.54296875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D9FE613-5FB5-4FCA-AD46-3B64AD01CDFC}">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -502,17 +402,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3">
+      <c r="A1" s="1">
         <v>4823957612</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3">
+      <c r="A2" s="1">
         <v>6324178059</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3">
+      <c r="A3" s="1">
         <v>2149867304</v>
       </c>
     </row>

</xml_diff>